<commit_message>
[IMP] 添加 0.19.0 changelog;修改 README.md;调整菜单顺序
</commit_message>
<xml_diff>
--- a/src/main/resources/script/meta/micro-service-init-data.xlsx
+++ b/src/main/resources/script/meta/micro-service-init-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540" tabRatio="500" activeTab="3"/>
+    <workbookView windowWidth="23955" windowHeight="11670" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
@@ -271,10 +271,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -320,6 +320,66 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -328,23 +388,63 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -356,93 +456,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -455,21 +470,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -480,13 +480,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -498,7 +564,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -510,157 +660,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -674,17 +674,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -719,7 +713,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -727,8 +721,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -748,15 +742,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -771,151 +756,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1445,8 +1445,8 @@
   <sheetPr/>
   <dimension ref="D7:P12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1509,7 +1509,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="4:15">
+    <row r="8" ht="15" spans="4:15">
       <c r="D8" s="4"/>
       <c r="F8" s="5" t="s">
         <v>36</v>
@@ -1540,7 +1540,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" ht="14.25" spans="6:15">
+    <row r="9" ht="15" spans="6:15">
       <c r="F9" s="5" t="s">
         <v>42</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" ht="14.25" spans="6:15">
+    <row r="10" ht="15" spans="6:15">
       <c r="F10" s="5" t="s">
         <v>47</v>
       </c>
@@ -1601,10 +1601,10 @@
         <v>49</v>
       </c>
       <c r="O10" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" ht="14.25" spans="6:15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="6:15">
       <c r="F11" s="5" t="s">
         <v>50</v>
       </c>
@@ -1633,10 +1633,10 @@
         <v>53</v>
       </c>
       <c r="O11" s="5">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" ht="14.25" spans="6:15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="6:15">
       <c r="F12" s="5" t="s">
         <v>54</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>57</v>
       </c>
       <c r="O12" s="5">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1715,7 +1715,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" ht="14.25" spans="4:7">
+    <row r="8" ht="15" spans="4:7">
       <c r="D8" s="4"/>
       <c r="F8" s="5" t="s">
         <v>42</v>
@@ -1724,7 +1724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" ht="14.25" spans="4:7">
+    <row r="9" ht="15" spans="4:7">
       <c r="D9" s="4"/>
       <c r="F9" s="5" t="s">
         <v>42</v>
@@ -1733,7 +1733,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" ht="14.25" spans="4:7">
+    <row r="10" ht="15" spans="4:7">
       <c r="D10" s="4"/>
       <c r="F10" s="5" t="s">
         <v>42</v>
@@ -1742,7 +1742,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" ht="14.25" spans="6:7">
+    <row r="11" ht="15" spans="6:7">
       <c r="F11" s="5" t="s">
         <v>47</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" ht="14.25" spans="6:7">
+    <row r="12" ht="15" spans="6:7">
       <c r="F12" s="5" t="s">
         <v>47</v>
       </c>
@@ -1758,7 +1758,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" ht="14.25" spans="6:7">
+    <row r="13" ht="15" spans="6:7">
       <c r="F13" s="5" t="s">
         <v>47</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" ht="14.25" spans="6:7">
+    <row r="14" ht="15" spans="6:7">
       <c r="F14" s="5" t="s">
         <v>50</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" ht="14.25" spans="6:7">
+    <row r="15" ht="15" spans="6:7">
       <c r="F15" s="5" t="s">
         <v>50</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" ht="14.25" spans="6:7">
+    <row r="16" ht="15" spans="6:7">
       <c r="F16" s="5" t="s">
         <v>50</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" ht="14.25" spans="6:7">
+    <row r="17" ht="15" spans="6:7">
       <c r="F17" s="5" t="s">
         <v>50</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" ht="14.25" spans="6:7">
+    <row r="18" ht="15" spans="6:7">
       <c r="F18" s="5" t="s">
         <v>50</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" ht="14.25" spans="6:7">
+    <row r="19" ht="15" spans="6:7">
       <c r="F19" s="5" t="s">
         <v>54</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" ht="14.25" spans="6:7">
+    <row r="20" ht="15" spans="6:7">
       <c r="F20" s="5" t="s">
         <v>54</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" ht="14.25" spans="6:7">
+    <row r="21" ht="15" spans="6:7">
       <c r="F21" s="5" t="s">
         <v>54</v>
       </c>
@@ -1845,7 +1845,7 @@
   <sheetPr/>
   <dimension ref="D4:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>